<commit_message>
Rettifica tripletta file eXcel di accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#EUROCHIMICASRLXX/EUROCHIMICA_SRL/EMAGING-RIS-GTW-CLIENT/1.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#EUROCHIMICASRLXX/EUROCHIMICA_SRL/EMAGING-RIS-GTW-CLIENT/1.1/report-checklist.xlsx
@@ -210,13 +210,13 @@
     <t xml:space="preserve">IDENTIFICATIVI SOFTWARE</t>
   </si>
   <si>
-    <t xml:space="preserve">subject_application_id: Emaging-RIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject_application_vendor: Eurochimica S.r.l.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject_application_version: 1.1.0</t>
+    <t xml:space="preserve">subject_application_id: Emaging-RIS-gtw-client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subject_application_vendor: Eurochimica Srl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subject_application_version: 1.1</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -3641,7 +3641,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="I26" activeCellId="0" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>